<commit_message>
Allow for alternative qualifying CES resource definition on web app
</commit_message>
<xml_diff>
--- a/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
+++ b/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\elec\RQSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\RQSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBD6EF5-C926-4C68-BE19-A8FF52319E8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RQSD-BRQSD" sheetId="2" r:id="rId2"/>
     <sheet name="RQSD-RQSD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Source:</t>
   </si>
@@ -140,9 +139,6 @@
     <t>local air quality, competing land use, and feedstock availability challenges.</t>
   </si>
   <si>
-    <t>as well as it may be useful for a more ambitious RE scenario with a delayed start.</t>
-  </si>
-  <si>
     <t>crude oil</t>
   </si>
   <si>
@@ -156,12 +152,18 @@
   </si>
   <si>
     <t>Qualifies for RPS (Boolean)</t>
+  </si>
+  <si>
+    <t>in addition to wind and solar as it may be useful for a more ambitious RE scenario with a delayed start.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro is not included due to potential state-level challenges in implementing additional capacity. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -319,23 +321,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -371,23 +356,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -563,28 +531,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="84.5703125" customWidth="1"/>
-    <col min="4" max="4" width="73.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.59765625" customWidth="1"/>
+    <col min="4" max="4" width="73.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>17</v>
@@ -604,7 +574,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="2">
         <v>2016</v>
       </c>
@@ -612,7 +582,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -620,7 +590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
@@ -628,89 +598,94 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{DD8F12BA-98DD-4700-833B-CFCD6A499337}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{78791D4D-6C5C-4031-BDF4-82843565F5BF}"/>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -718,166 +693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <f>B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -887,21 +703,21 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.86328125" customWidth="1"/>
+    <col min="2" max="2" width="27.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -909,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -917,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -925,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -933,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -941,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -949,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -957,23 +773,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -981,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -989,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -998,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1006,25 +822,184 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>37</v>
       </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.3984375" customWidth="1"/>
+    <col min="2" max="2" width="32.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
       <c r="B15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>38</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>39</v>
       </c>
       <c r="B17">
         <v>1</v>

</xml_diff>